<commit_message>
Trabajo en el script 7 pasando todos los datos de salarios reales a numeros indice para poder compararlos mejor. De todas formas, esto tiene limitaciones porque el año 2025 no esta completo.
</commit_message>
<xml_diff>
--- a/DATOS/RESULTADOS/salario_real_oficial_ccaa.xlsx
+++ b/DATOS/RESULTADOS/salario_real_oficial_ccaa.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,25 +406,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>11.60820569701307</v>
+        <v>11.60260019864755</v>
       </c>
       <c r="C2">
-        <v>12.35527625760794</v>
+        <v>12.33368594715992</v>
       </c>
       <c r="D2">
-        <v>11.98378132164803</v>
+        <v>11.967846525</v>
       </c>
       <c r="E2">
-        <v>11.20288928277543</v>
+        <v>11.18011887873801</v>
       </c>
       <c r="F2">
-        <v>11.31782864175056</v>
+        <v>11.25746539402369</v>
       </c>
       <c r="G2">
-        <v>11.36559885105061</v>
+        <v>11.31191657662111</v>
       </c>
       <c r="H2">
-        <v>11.15957711465343</v>
+        <v>11.0948433886587</v>
       </c>
     </row>
     <row r="3">
@@ -434,25 +434,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>12.58316662627527</v>
+        <v>12.59231637119373</v>
       </c>
       <c r="C3">
-        <v>12.91248955846217</v>
+        <v>12.94189373991007</v>
       </c>
       <c r="D3">
-        <v>12.67981508557311</v>
+        <v>12.6781539651283</v>
       </c>
       <c r="E3">
-        <v>11.8791733862533</v>
+        <v>11.83621986310745</v>
       </c>
       <c r="F3">
-        <v>12.01132304381861</v>
+        <v>12.03783229194669</v>
       </c>
       <c r="G3">
-        <v>12.17950362810794</v>
+        <v>12.20090987489004</v>
       </c>
       <c r="H3">
-        <v>11.78971717030781</v>
+        <v>11.79205809379728</v>
       </c>
     </row>
     <row r="4">
@@ -462,25 +462,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>13.45692907933558</v>
+        <v>13.4667622838789</v>
       </c>
       <c r="C4">
-        <v>14.10368777051056</v>
+        <v>14.13864366746315</v>
       </c>
       <c r="D4">
-        <v>13.74546677930668</v>
+        <v>13.799922375</v>
       </c>
       <c r="E4">
-        <v>12.69911260975097</v>
+        <v>12.7721133334717</v>
       </c>
       <c r="F4">
-        <v>12.84138249737083</v>
+        <v>12.93852660929048</v>
       </c>
       <c r="G4">
-        <v>13.04531559757965</v>
+        <v>13.13300537461461</v>
       </c>
       <c r="H4">
-        <v>12.30602547397301</v>
+        <v>12.36535599334476</v>
       </c>
     </row>
     <row r="5">
@@ -490,25 +490,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>11.77357881666008</v>
+        <v>11.77925334390886</v>
       </c>
       <c r="C5">
-        <v>12.74408731642623</v>
+        <v>12.7458725529953</v>
       </c>
       <c r="D5">
-        <v>12.25259436150875</v>
+        <v>12.2383543236286</v>
       </c>
       <c r="E5">
-        <v>11.42831731726805</v>
+        <v>11.46529868898703</v>
       </c>
       <c r="F5">
-        <v>11.75526357228579</v>
+        <v>11.75750587755254</v>
       </c>
       <c r="G5">
-        <v>12.02378205086483</v>
+        <v>12.00597498558663</v>
       </c>
       <c r="H5">
-        <v>11.91574518143869</v>
+        <v>11.84818824381014</v>
       </c>
     </row>
     <row r="6">
@@ -518,25 +518,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>10.98620530669895</v>
+        <v>11.04136413156123</v>
       </c>
       <c r="C6">
-        <v>11.73367386421054</v>
+        <v>11.68963463147117</v>
       </c>
       <c r="D6">
-        <v>11.29494790700493</v>
+        <v>11.3585287154406</v>
       </c>
       <c r="E6">
-        <v>10.61058817253992</v>
+        <v>10.77479266543566</v>
       </c>
       <c r="F6">
-        <v>10.59019297681147</v>
+        <v>10.64941057978176</v>
       </c>
       <c r="G6">
-        <v>10.68457648657407</v>
+        <v>10.74454439942906</v>
       </c>
       <c r="H6">
-        <v>10.43186698586546</v>
+        <v>10.54267422872699</v>
       </c>
     </row>
     <row r="7">
@@ -546,25 +546,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>12.51158721627881</v>
+        <v>12.52136834631571</v>
       </c>
       <c r="C7">
-        <v>13.02640872219237</v>
+        <v>13.03817355621505</v>
       </c>
       <c r="D7">
-        <v>12.4206025114217</v>
+        <v>12.42311535259613</v>
       </c>
       <c r="E7">
-        <v>11.83497181086259</v>
+        <v>11.87366646679993</v>
       </c>
       <c r="F7">
-        <v>11.8619550187578</v>
+        <v>11.87617869085521</v>
       </c>
       <c r="G7">
-        <v>11.95526455687786</v>
+        <v>11.98882425984096</v>
       </c>
       <c r="H7">
-        <v>11.37097893977618</v>
+        <v>11.42292719915424</v>
       </c>
     </row>
     <row r="8">
@@ -574,25 +574,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>11.92661065872148</v>
+        <v>11.92937655860349</v>
       </c>
       <c r="C8">
-        <v>12.43452437150721</v>
+        <v>12.46490140278902</v>
       </c>
       <c r="D8">
-        <v>12.16619017012495</v>
+        <v>12.156855975</v>
       </c>
       <c r="E8">
-        <v>11.50345999543226</v>
+        <v>11.40461087454539</v>
       </c>
       <c r="F8">
-        <v>11.66564275724931</v>
+        <v>11.5807511907452</v>
       </c>
       <c r="G8">
-        <v>11.78085639036557</v>
+        <v>11.71345400159246</v>
       </c>
       <c r="H8">
-        <v>11.50920321004876</v>
+        <v>11.44121022945437</v>
       </c>
     </row>
     <row r="9">
@@ -602,25 +602,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>11.59586441942747</v>
+        <v>11.58063773081721</v>
       </c>
       <c r="C9">
-        <v>12.15715597285976</v>
+        <v>12.16988072206184</v>
       </c>
       <c r="D9">
-        <v>11.97898108879338</v>
+        <v>11.93286706905589</v>
       </c>
       <c r="E9">
-        <v>11.22941022800986</v>
+        <v>11.03170125288324</v>
       </c>
       <c r="F9">
-        <v>11.27088440530288</v>
+        <v>11.07281577020706</v>
       </c>
       <c r="G9">
-        <v>11.40712460498211</v>
+        <v>11.21224091020639</v>
       </c>
       <c r="H9">
-        <v>11.14331543579783</v>
+        <v>10.96747645961166</v>
       </c>
     </row>
     <row r="10">
@@ -630,25 +630,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>14.02709610379019</v>
+        <v>14.01261739635469</v>
       </c>
       <c r="C10">
-        <v>14.74510219238277</v>
+        <v>14.74228291531547</v>
       </c>
       <c r="D10">
-        <v>14.38149763254857</v>
+        <v>14.41524198729834</v>
       </c>
       <c r="E10">
-        <v>13.50137120309235</v>
+        <v>13.60834283068732</v>
       </c>
       <c r="F10">
-        <v>13.73545681880625</v>
+        <v>13.86919613336777</v>
       </c>
       <c r="G10">
-        <v>13.87998325160273</v>
+        <v>14.0061547047694</v>
       </c>
       <c r="H10">
-        <v>13.51752054871499</v>
+        <v>13.65358531443892</v>
       </c>
     </row>
     <row r="11">
@@ -658,25 +658,25 @@
         </is>
       </c>
       <c r="B11">
-        <v>11.9537614694098</v>
+        <v>11.96245767122055</v>
       </c>
       <c r="C11">
-        <v>12.51129598184712</v>
+        <v>12.52913047146017</v>
       </c>
       <c r="D11">
-        <v>12.290996224346</v>
+        <v>12.29499865416779</v>
       </c>
       <c r="E11">
-        <v>11.50345999543226</v>
+        <v>11.52187616689947</v>
       </c>
       <c r="F11">
-        <v>11.74672825656803</v>
+        <v>11.77064616174712</v>
       </c>
       <c r="G11">
-        <v>11.93450167991211</v>
+        <v>11.96075867871859</v>
       </c>
       <c r="H11">
-        <v>11.57831534518505</v>
+        <v>11.57075624929744</v>
       </c>
     </row>
     <row r="12">
@@ -686,25 +686,25 @@
         </is>
       </c>
       <c r="B12">
-        <v>10.88747508601417</v>
+        <v>10.89174287932444</v>
       </c>
       <c r="C12">
-        <v>11.19627259183112</v>
+        <v>11.18313488420164</v>
       </c>
       <c r="D12">
-        <v>11.17734220206587</v>
+        <v>11.14584952641588</v>
       </c>
       <c r="E12">
-        <v>10.48240360390686</v>
+        <v>10.41962370921107</v>
       </c>
       <c r="F12">
-        <v>10.50483981963387</v>
+        <v>10.48201131607158</v>
       </c>
       <c r="G12">
-        <v>10.90881555780415</v>
+        <v>10.8828572561911</v>
       </c>
       <c r="H12">
-        <v>10.72051178555231</v>
+        <v>10.67089705020983</v>
       </c>
     </row>
     <row r="13">
@@ -714,25 +714,25 @@
         </is>
       </c>
       <c r="B13">
-        <v>11.95622972492692</v>
+        <v>11.95100758960922</v>
       </c>
       <c r="C13">
-        <v>12.53358451388129</v>
+        <v>12.52890557923256</v>
       </c>
       <c r="D13">
-        <v>12.32219773790126</v>
+        <v>12.27911615</v>
       </c>
       <c r="E13">
-        <v>11.48798944404551</v>
+        <v>11.40159626372215</v>
       </c>
       <c r="F13">
-        <v>11.58882491578946</v>
+        <v>11.49929374661104</v>
       </c>
       <c r="G13">
-        <v>11.92827281682239</v>
+        <v>11.81589671469163</v>
       </c>
       <c r="H13">
-        <v>11.65555831974913</v>
+        <v>11.57171436027681</v>
       </c>
     </row>
     <row r="14">
@@ -742,25 +742,25 @@
         </is>
       </c>
       <c r="B14">
-        <v>14.8638347240937</v>
+        <v>14.89118209854162</v>
       </c>
       <c r="C14">
-        <v>15.9239178866344</v>
+        <v>15.95645235579862</v>
       </c>
       <c r="D14">
-        <v>15.36074513489834</v>
+        <v>15.45918711734407</v>
       </c>
       <c r="E14">
-        <v>14.41192365614097</v>
+        <v>14.64623406208957</v>
       </c>
       <c r="F14">
-        <v>14.76609619172585</v>
+        <v>15.08291186356561</v>
       </c>
       <c r="G14">
-        <v>15.00740747084286</v>
+        <v>15.34078644749878</v>
       </c>
       <c r="H14">
-        <v>14.48102502090911</v>
+        <v>14.79103938427232</v>
       </c>
     </row>
     <row r="15">
@@ -770,25 +770,25 @@
         </is>
       </c>
       <c r="B15">
-        <v>11.30954677944161</v>
+        <v>11.30672076401736</v>
       </c>
       <c r="C15">
-        <v>11.968941702349</v>
+        <v>11.95675404627403</v>
       </c>
       <c r="D15">
-        <v>11.75097002819723</v>
+        <v>11.76079419933817</v>
       </c>
       <c r="E15">
-        <v>11.01945274490399</v>
+        <v>11.00712111789826</v>
       </c>
       <c r="F15">
-        <v>11.28582120780896</v>
+        <v>11.25576283749813</v>
       </c>
       <c r="G15">
-        <v>11.60644822385329</v>
+        <v>11.58549535169647</v>
       </c>
       <c r="H15">
-        <v>11.22055841036191</v>
+        <v>11.25198932239388</v>
       </c>
     </row>
     <row r="16">
@@ -798,25 +798,25 @@
         </is>
       </c>
       <c r="B16">
-        <v>14.66884253824126</v>
+        <v>14.62933733082327</v>
       </c>
       <c r="C16">
-        <v>15.42366416764527</v>
+        <v>15.42078682931872</v>
       </c>
       <c r="D16">
-        <v>14.72951451451111</v>
+        <v>14.69858752382294</v>
       </c>
       <c r="E16">
-        <v>14.02515987147226</v>
+        <v>13.96784545364735</v>
       </c>
       <c r="F16">
-        <v>14.19636386756533</v>
+        <v>14.12999791611706</v>
       </c>
       <c r="G16">
-        <v>14.38244487417384</v>
+        <v>14.3395125069415</v>
       </c>
       <c r="H16">
-        <v>13.83055786668523</v>
+        <v>13.79513149636294</v>
       </c>
     </row>
     <row r="17">
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="B17">
-        <v>16.34725628988253</v>
+        <v>16.29310739315033</v>
       </c>
       <c r="C17">
-        <v>17.28104183715939</v>
+        <v>17.19013484234888</v>
       </c>
       <c r="D17">
-        <v>16.36399380152139</v>
+        <v>16.29247682706402</v>
       </c>
       <c r="E17">
-        <v>15.4219296538187</v>
+        <v>15.4326069921872</v>
       </c>
       <c r="F17">
-        <v>15.58335267170142</v>
+        <v>15.58695838087561</v>
       </c>
       <c r="G17">
-        <v>15.60330203975984</v>
+        <v>15.56313738617234</v>
       </c>
       <c r="H17">
-        <v>15.0745762991384</v>
+        <v>14.98580102321255</v>
       </c>
     </row>
     <row r="18">
@@ -854,53 +854,25 @@
         </is>
       </c>
       <c r="B18">
-        <v>12.11419807802257</v>
+        <v>12.09773894536583</v>
       </c>
       <c r="C18">
-        <v>12.59797360642445</v>
+        <v>12.61083418147217</v>
       </c>
       <c r="D18">
-        <v>12.29339634077332</v>
+        <v>12.29918200136333</v>
       </c>
       <c r="E18">
-        <v>11.46367857758062</v>
+        <v>11.43500496148252</v>
       </c>
       <c r="F18">
-        <v>11.74459442763859</v>
+        <v>11.72513991261468</v>
       </c>
       <c r="G18">
-        <v>11.89712850137377</v>
+        <v>11.88401368990424</v>
       </c>
       <c r="H18">
-        <v>11.66775457889083</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Total Nacional</t>
-        </is>
-      </c>
-      <c r="B19">
-        <v>13.0546034300451</v>
-      </c>
-      <c r="C19">
-        <v>13.81393685406636</v>
-      </c>
-      <c r="D19">
-        <v>13.42145106161742</v>
-      </c>
-      <c r="E19">
-        <v>12.56650788357883</v>
-      </c>
-      <c r="F19">
-        <v>12.76456465591098</v>
-      </c>
-      <c r="G19">
-        <v>12.93734863735776</v>
-      </c>
-      <c r="H19">
-        <v>12.58653943423206</v>
+        <v>11.67685402695732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>